<commit_message>
Added Icon Support topicslist.json
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\03_mindoffwork-posts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A2711A6F-5695-487C-ACDC-62A5CB4572DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5C9F5A43-E20C-4A80-8A18-EE5C6A527996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
@@ -35,18 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>SLUG</t>
-  </si>
-  <si>
-    <t>SRC</t>
-  </si>
-  <si>
-    <t>ALT</t>
+    <t>NAME</t>
   </si>
   <si>
     <t>TOPIC</t>
@@ -55,9 +49,6 @@
     <t>COLOR</t>
   </si>
   <si>
-    <t>POST</t>
-  </si>
-  <si>
     <t>DESCRIPTION</t>
   </si>
   <si>
@@ -79,36 +70,6 @@
     <t>Food</t>
   </si>
   <si>
-    <t>&lt;path d="m352-522 86-87-56-57-44 44-56-56 43-44-45-45-87 87 159 158Zm328 329 87-87-45-45-44 43-56-56 43-44-57-56-86 86 158 159Zm24-567 57 57-57-57ZM290-120H120v-170l175-175L80-680l200-200 216 216 151-152q12-12 27-18t31-6q16 0 31 6t27 18l53 54q12 12 18 27t6 31q0 16-6 30.5T816-647L665-495l215 215L680-80 465-295 290-120Zm-90-80h56l392-391-57-57-391 392v56Zm420-419-29-29 57 57-28-28Z" /&gt;</t>
-  </si>
-  <si>
-    <t>&lt;path d="M756-120 537-339l84-84 219 219-84 84Zm-552 0-84-84 276-276-68-68-28 28-51-51v82l-28 28-121-121 28-28h82l-50-50 142-142q20-20 43-29t47-9q24 0 47 9t43 29l-92 92 50 50-28 28 68 68 90-90q-4-11-6.5-23t-2.5-24q0-59 40.5-99.5T701-841q15 0 28.5 3t27.5 9l-99 99 72 72 99-99q7 14 9.5 27.5T841-701q0 59-40.5 99.5T701-561q-12 0-24-2t-23-7L204-120Z" /&gt;</t>
-  </si>
-  <si>
-    <t>&lt;path d="M480-80q-73-9-145-39.5T206.5-207Q150-264 115-351T80-560v-40h40q51 0 105 13t101 39q12-86 54.5-176.5T480-880q57 65 99.5 155.5T634-548q47-26 101-39t105-13h40v40q0 122-35 209t-91.5 144q-56.5 57-128 87.5T480-80Zm-2-82q-11-166-98.5-251T162-518q11 171 101.5 255T478-162Zm2-254q15-22 36.5-45.5T558-502q-2-57-22.5-119T480-742q-35 59-55.5 121T402-502q20 17 42 40.5t36 45.5Zm78 236q37-12 77-35t74.5-62.5q34.5-39.5 59-98.5T798-518q-94 14-165 62.5T524-332q12 32 20.5 70t13.5 82Zm-78-236Zm78 236Zm-80 18Zm46-170ZM480-80Z" /&gt;</t>
-  </si>
-  <si>
-    <t>&lt;path d="M272-160q-30 0-51-21t-21-51q0-21 12-39.5t32-26.5l156-62v-90q-54 63-125.5 96.5T120-320v-80q68 0 123.5-28T344-508l54-64q12-14 28-21t34-7h40q18 0 34 7t28 21l54 64q45 52 100.5 80T840-400v80q-83 0-154.5-33.5T560-450v90l156 62q20 8 32 26.5t12 39.5q0 30-21 51t-51 21H400v-20q0-26 17-43t43-17h120q9 0 14.5-5.5T600-260q0-9-5.5-14.5T580-280H460q-42 0-71 29t-29 71v20h-88Zm208-480q-33 0-56.5-23.5T400-720q0-33 23.5-56.5T480-800q33 0 56.5 23.5T560-720q0 33-23.5 56.5T480-640Z" /&gt;</t>
-  </si>
-  <si>
-    <t>&lt;path d="M400-120q-66 0-113-47t-47-113q0-66 47-113t113-47q23 0 42.5 5.5T480-418v-422h240v160H560v400q0 66-47 113t-113 47Z" /&gt;</t>
-  </si>
-  <si>
-    <t>&lt;path d="M280-80v-366q-51-14-85.5-56T160-600v-280h80v280h40v-280h80v280h40v-280h80v280q0 56-34.5 98T360-446v366h-80Zm400 0v-320H560v-280q0-83 58.5-141.5T760-880v800h-80Z" /&gt;</t>
-  </si>
-  <si>
-    <t>&lt;path d="M320-240 80-480l240-240 57 57-184 184 183 183-56 56Zm320 0-57-57 184-184-183-183 56-56 240 240-240 240Z" /&gt;</t>
-  </si>
-  <si>
-    <t>&lt;path d="M80-160v-120h80v-440q0-33 23.5-56.5T240-800h600v80H240v440h240v120H80Zm520 0q-17 0-28.5-11.5T560-200v-400q0-17 11.5-28.5T600-640h240q17 0 28.5 11.5T880-600v400q0 17-11.5 28.5T840-160H600Zm40-120h160v-280H640v280Zm0 0h160-160Z" /&gt;</t>
-  </si>
-  <si>
-    <t>&lt;path d="M342-160h276l40-160H302l40 160Zm0 80q-28 0-49-17t-28-44l-45-179h520l-45 179q-7 27-28 44t-49 17H342ZM200-400h560v-80H200v80Zm280-240q0-100 70-170t170-70q0 90-57 156t-143 80v84h320v160q0 33-23.5 56.5T760-320H200q-33 0-56.5-23.5T120-400v-160h320v-84q-86-14-143-80t-57-156q100 0 170 70t70 170Z" /&gt;</t>
-  </si>
-  <si>
-    <t>&lt;path d="M180-475q-42 0-71-29t-29-71q0-42 29-71t71-29q42 0 71 29t29 71q0 42-29 71t-71 29Zm180-160q-42 0-71-29t-29-71q0-42 29-71t71-29q42 0 71 29t29 71q0 42-29 71t-71 29Zm240 0q-42 0-71-29t-29-71q0-42 29-71t71-29q42 0 71 29t29 71q0 42-29 71t-71 29Zm180 160q-42 0-71-29t-29-71q0-42 29-71t71-29q42 0 71 29t29 71q0 42-29 71t-71 29ZM266-75q-45 0-75.5-34.5T160-191q0-52 35.5-91t70.5-77q29-31 50-67.5t50-68.5q22-26 51-43t63-17q34 0 63 17t51 43q25 30 50 68.5t50 67.5q35 35 70.5 77t35.5 91q0 52-30.5 86.5T430-75Zm-26-173h120v80H240v-80Z" /&gt;</t>
-  </si>
-  <si>
     <t>Programming</t>
   </si>
   <si>
@@ -119,6 +80,48 @@
   </si>
   <si>
     <t>Pets</t>
+  </si>
+  <si>
+    <t>design_services</t>
+  </si>
+  <si>
+    <t>ICON</t>
+  </si>
+  <si>
+    <t>LINK</t>
+  </si>
+  <si>
+    <t>IMG</t>
+  </si>
+  <si>
+    <t>IMG_ALT</t>
+  </si>
+  <si>
+    <t>construction</t>
+  </si>
+  <si>
+    <t>spa</t>
+  </si>
+  <si>
+    <t>self_improvement</t>
+  </si>
+  <si>
+    <t>palette</t>
+  </si>
+  <si>
+    <t>restaurant</t>
+  </si>
+  <si>
+    <t>developer_mode</t>
+  </si>
+  <si>
+    <t>devices</t>
+  </si>
+  <si>
+    <t>park</t>
+  </si>
+  <si>
+    <t>pets</t>
   </si>
 </sst>
 </file>
@@ -506,7 +509,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -515,7 +518,8 @@
     <col min="2" max="2" width="30.90625" style="2" customWidth="1"/>
     <col min="3" max="3" width="8.7265625" style="2"/>
     <col min="4" max="4" width="29" style="2" customWidth="1"/>
-    <col min="5" max="7" width="8.7265625" style="2"/>
+    <col min="5" max="5" width="9.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.7265625" style="2"/>
     <col min="8" max="8" width="57.26953125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -524,25 +528,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -567,7 +571,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -583,13 +587,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -597,14 +601,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>LOWER(B2)</f>
         <v>design</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -613,14 +617,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="str">
         <f t="shared" ref="C3:C11" si="0">LOWER(B3)</f>
         <v>build</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -629,14 +633,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>philosophy</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -645,14 +649,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>lifestyle</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -661,14 +665,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>artistry</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -677,14 +681,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>food</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -693,14 +697,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>programming</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -709,14 +713,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>tech</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -725,14 +729,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>gardening</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -741,14 +745,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>pets</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added topic wise post generation to spreadjsoninator
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\03_mindoffwork-posts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5C9F5A43-E20C-4A80-8A18-EE5C6A527996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D5D222-72C9-41D0-935C-747CDB24AD61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
   <sheets>
     <sheet name="posts" sheetId="1" r:id="rId1"/>
     <sheet name="topics" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -122,6 +123,129 @@
   </si>
   <si>
     <t>pets</t>
+  </si>
+  <si>
+    <t>Explore the art of minimalistic design, where every element serves a purpose. Discover how simplicity can lead to elegance in aesthetics and functionality, transforming spaces into serene environments that inspire creativity and clarity.</t>
+  </si>
+  <si>
+    <t>Dive into the art of building with a focus on efficiency and purposeful creation. Learn how to construct meaningful structures using sustainable materials and techniques, embracing essentialism while respecting both nature and your time.</t>
+  </si>
+  <si>
+    <t>Engage with profound ideas that encourage intentional living and a deeper understanding of life’s complexities. Explore philosophical concepts that inspire you to embrace simplicity and find beauty in the everyday, often drawing from minimalistic principles.</t>
+  </si>
+  <si>
+    <t>Embrace a lifestyle centered around mindful choices and meaningful experiences. Discover practical tips for decluttering your environment, prioritizing what truly matters, and cultivating a life rich in joy and fulfillment, reflecting essentialist values.</t>
+  </si>
+  <si>
+    <t>Celebrate the beauty of simplicity in artistic expression. Explore how a refined approach, rooted in minimalism, can elevate your creativity, allowing you to connect deeply with your audience and convey powerful messages through your work.</t>
+  </si>
+  <si>
+    <t>Savor the art of cooking with straightforward recipes that emphasize quality ingredients and simple techniques. Empower yourself to create nourishing meals that delight the senses while minimizing clutter in your kitchen.</t>
+  </si>
+  <si>
+    <t>Unlock the power of efficient coding practices that embrace clarity and simplicity. Learn how to write clean, streamlined code that enhances functionality, allowing you to tackle challenges with a minimalistic mindset.</t>
+  </si>
+  <si>
+    <t>Navigate the tech landscape with a focus on practical tools and innovations. Discover how to enhance productivity while reducing distractions, empowering you to use technology effectively in your daily life, all while keeping things essential.</t>
+  </si>
+  <si>
+    <t>Celebrate the joy of pet ownership with a thoughtful approach. Learn how to provide a loving, uncomplicated environment for your pets, focusing on their needs while enjoying a harmonious home that enhances your bond with them.</t>
+  </si>
+  <si>
+    <t>Cultivate a garden that reflects your passion for nature and simplicity. Discover strategies for creating beautiful, low-maintenance spaces that promote sustainability and deepen your connection to the environment.</t>
+  </si>
+  <si>
+    <t>The Art of Minimalism in Modern Design</t>
+  </si>
+  <si>
+    <t>Explore how minimalism influences contemporary design choices, from architecture to interior decor. Discover practical tips for incorporating minimalistic principles to create serene and functional spaces that prioritize simplicity and usability.</t>
+  </si>
+  <si>
+    <t>DIY Projects: Crafting Functional Furniture from Reclaimed Wood</t>
+  </si>
+  <si>
+    <t>Dive into the world of DIY furniture building using reclaimed wood. This post outlines essential tools and techniques, plus step-by-step guides to create beautiful, sustainable pieces that enhance your living space while reducing waste.</t>
+  </si>
+  <si>
+    <t>This post delves into how philosophical ideas shape our understanding of design. Explore concepts like functionality, aesthetics, and emotional connection, and learn how to create spaces that reflect deeper values and purpose.</t>
+  </si>
+  <si>
+    <t>Discover the benefits of decluttering your home and mind for a simpler lifestyle. This post offers practical strategies to reduce excess, create organized spaces, and cultivate a more intentional approach to daily living.</t>
+  </si>
+  <si>
+    <t>This post encourages readers to embrace their creativity, regardless of skill level. Learn how to explore different artistic mediums, overcome creative blocks, and find inspiration in everyday life to express your unique artistic voice.</t>
+  </si>
+  <si>
+    <t>This post presents easy, nutritious recipes designed for those with a hectic schedule. Discover meal prep tips and quick dishes that prioritize healthy ingredients without sacrificing flavor, making it easier to eat well daily.</t>
+  </si>
+  <si>
+    <t>Explore essential coding practices that lead to cleaner, more maintainable code. This post covers topics such as code organization, commenting, and utilizing frameworks to enhance efficiency and readability in programming projects.</t>
+  </si>
+  <si>
+    <t>Discover how smart home technology is revolutionizing the way we live. This post explores the latest advancements in home automation, security, and energy efficiency, offering tips on creating a connected and convenient living environment.</t>
+  </si>
+  <si>
+    <t>This post is a beginner's guide to starting a sustainable garden at home. Learn about essential plants, soil preparation, and eco-friendly practices that promote biodiversity and help you grow your own food and flowers.</t>
+  </si>
+  <si>
+    <t>Explore the fascinating world of pet behavior and communication. This post offers insights into understanding your pet's needs and emotions, providing tips for strengthening the bond between you and your animal companions through positive reinforcement and care.</t>
+  </si>
+  <si>
+    <t>Understanding Pet Behavior: Building a Stronger Bond with Your Furry Friends</t>
+  </si>
+  <si>
+    <t>Gardening for Beginners: Cultivating a Sustainable Home Garden</t>
+  </si>
+  <si>
+    <t>The Future of Smart Homes: Integrating Technology for a Seamless Lifestyle</t>
+  </si>
+  <si>
+    <t>Streamlining Your Code: Best Practices for Clean Programming</t>
+  </si>
+  <si>
+    <t>Nourishing Simplicity: Wholesome Recipes for Busy Lives</t>
+  </si>
+  <si>
+    <t>The Joy of Creating: Finding Your Artistic Voice</t>
+  </si>
+  <si>
+    <t>Simplifying Your Life: The Power of Decluttering</t>
+  </si>
+  <si>
+    <t>cartoon-illustration-of-small-pond-with-lillypads-and-lotus-in-the-middle-surrounded-by-stones-and-plants-with-lavender-background.jpeg</t>
+  </si>
+  <si>
+    <t>#152523</t>
+  </si>
+  <si>
+    <t>UPDATED_ON</t>
+  </si>
+  <si>
+    <t>design</t>
+  </si>
+  <si>
+    <t>build</t>
+  </si>
+  <si>
+    <t>philosophy</t>
+  </si>
+  <si>
+    <t>lifestyle</t>
+  </si>
+  <si>
+    <t>artistry</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>programming</t>
+  </si>
+  <si>
+    <t>tech</t>
+  </si>
+  <si>
+    <t>gardening</t>
   </si>
 </sst>
 </file>
@@ -159,7 +283,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -167,31 +291,23 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,253 +622,614 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE75069E-C97D-4B74-95E9-9740559F44A7}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="2"/>
-    <col min="2" max="2" width="30.90625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="2"/>
-    <col min="4" max="4" width="29" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.7265625" style="2"/>
-    <col min="8" max="8" width="57.26953125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="30.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="29" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="1"/>
+    <col min="6" max="6" width="57.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="1"/>
+    <col min="8" max="8" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
+      <c r="I1" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
+      <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="1" t="str">
+        <f>LOWER(SUBSTITUTE(B2, " ", "-"))</f>
+        <v>the-art-of-minimalism-in-modern-design</v>
+      </c>
+      <c r="H2" s="4" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(D2, "-", " "), ".", " ")</f>
+        <v>cartoon illustration of small pond with lillypads and lotus in the middle surrounded by stones and plants with lavender background jpeg</v>
+      </c>
+      <c r="I2" s="7">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
         <f>A2+1</f>
         <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="1" t="str">
+        <f>LOWER(SUBSTITUTE(B3, " ", "-"))</f>
+        <v>diy-projects:-crafting-functional-furniture-from-reclaimed-wood</v>
+      </c>
+      <c r="H3" s="4" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(D3, "-", " "), ".", " ")</f>
+        <v>cartoon illustration of small pond with lillypads and lotus in the middle surrounded by stones and plants with lavender background jpeg</v>
+      </c>
+      <c r="I3" s="7">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <f t="shared" ref="A4:A11" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="1" t="str">
+        <f>LOWER(SUBSTITUTE(B4, " ", "-"))</f>
+        <v>dive-into-the-world-of-diy-furniture-building-using-reclaimed-wood.-this-post-outlines-essential-tools-and-techniques,-plus-step-by-step-guides-to-create-beautiful,-sustainable-pieces-that-enhance-your-living-space-while-reducing-waste.</v>
+      </c>
+      <c r="H4" s="4" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(D4, "-", " "), ".", " ")</f>
+        <v>cartoon illustration of small pond with lillypads and lotus in the middle surrounded by stones and plants with lavender background jpeg</v>
+      </c>
+      <c r="I4" s="7">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="1" t="str">
+        <f>LOWER(SUBSTITUTE(B5, " ", "-"))</f>
+        <v>simplifying-your-life:-the-power-of-decluttering</v>
+      </c>
+      <c r="H5" s="4" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(D5, "-", " "), ".", " ")</f>
+        <v>cartoon illustration of small pond with lillypads and lotus in the middle surrounded by stones and plants with lavender background jpeg</v>
+      </c>
+      <c r="I5" s="7">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <f>LOWER(SUBSTITUTE(B6, " ", "-"))</f>
+        <v>the-joy-of-creating:-finding-your-artistic-voice</v>
+      </c>
+      <c r="H6" s="4" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(D6, "-", " "), ".", " ")</f>
+        <v>cartoon illustration of small pond with lillypads and lotus in the middle surrounded by stones and plants with lavender background jpeg</v>
+      </c>
+      <c r="I6" s="7">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="1" t="str">
+        <f>LOWER(SUBSTITUTE(B7, " ", "-"))</f>
+        <v>nourishing-simplicity:-wholesome-recipes-for-busy-lives</v>
+      </c>
+      <c r="H7" s="4" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(D7, "-", " "), ".", " ")</f>
+        <v>cartoon illustration of small pond with lillypads and lotus in the middle surrounded by stones and plants with lavender background jpeg</v>
+      </c>
+      <c r="I7" s="7">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <f>LOWER(SUBSTITUTE(B8, " ", "-"))</f>
+        <v>streamlining-your-code:-best-practices-for-clean-programming</v>
+      </c>
+      <c r="H8" s="4" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(D8, "-", " "), ".", " ")</f>
+        <v>cartoon illustration of small pond with lillypads and lotus in the middle surrounded by stones and plants with lavender background jpeg</v>
+      </c>
+      <c r="I8" s="7">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="1" t="str">
+        <f>LOWER(SUBSTITUTE(B9, " ", "-"))</f>
+        <v>the-future-of-smart-homes:-integrating-technology-for-a-seamless-lifestyle</v>
+      </c>
+      <c r="H9" s="4" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(D9, "-", " "), ".", " ")</f>
+        <v>cartoon illustration of small pond with lillypads and lotus in the middle surrounded by stones and plants with lavender background jpeg</v>
+      </c>
+      <c r="I9" s="7">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="1" t="str">
+        <f>LOWER(SUBSTITUTE(B10, " ", "-"))</f>
+        <v>gardening-for-beginners:-cultivating-a-sustainable-home-garden</v>
+      </c>
+      <c r="H10" s="4" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(D10, "-", " "), ".", " ")</f>
+        <v>cartoon illustration of small pond with lillypads and lotus in the middle surrounded by stones and plants with lavender background jpeg</v>
+      </c>
+      <c r="I10" s="7">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="1" t="str">
+        <f>LOWER(SUBSTITUTE(B11, " ", "-"))</f>
+        <v>understanding-pet-behavior:-building-a-stronger-bond-with-your-furry-friends</v>
+      </c>
+      <c r="H11" s="4" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(D11, "-", " "), ".", " ")</f>
+        <v>cartoon illustration of small pond with lillypads and lotus in the middle surrounded by stones and plants with lavender background jpeg</v>
+      </c>
+      <c r="I11" s="7">
+        <v>45576</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{68ECA381-B367-4D59-A9C6-BF1895F31450}">
+          <x14:formula1>
+            <xm:f>topics!$C$2:$C$1000</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C11</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8A1887-075D-436C-B79D-D9001D13C034}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="2"/>
-    <col min="2" max="2" width="26.90625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.453125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="4"/>
+    <col min="2" max="2" width="26.90625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.453125" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="str">
+      <c r="C2" s="6" t="str">
         <f>LOWER(B2)</f>
         <v>design</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
+      <c r="E2" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="str">
+      <c r="C3" s="6" t="str">
         <f t="shared" ref="C3:C11" si="0">LOWER(B3)</f>
         <v>build</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+      <c r="E3" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
         <f>A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="str">
+      <c r="C4" s="6" t="str">
         <f t="shared" si="0"/>
         <v>philosophy</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+      <c r="E4" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
         <f>A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="str">
+      <c r="C5" s="6" t="str">
         <f t="shared" si="0"/>
         <v>lifestyle</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+      <c r="E5" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
         <f>A5+1</f>
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="str">
+      <c r="C6" s="6" t="str">
         <f t="shared" si="0"/>
         <v>artistry</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+      <c r="E6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
         <f>A6+1</f>
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2" t="str">
+      <c r="C7" s="6" t="str">
         <f t="shared" si="0"/>
         <v>food</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+      <c r="E7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
         <f t="shared" ref="A8:A11" si="1">A7+1</f>
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2" t="str">
+      <c r="C8" s="6" t="str">
         <f t="shared" si="0"/>
         <v>programming</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="2" t="str">
+      <c r="C9" s="6" t="str">
         <f t="shared" si="0"/>
         <v>tech</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
+      <c r="E9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="2" t="str">
+      <c r="C10" s="6" t="str">
         <f t="shared" si="0"/>
         <v>gardening</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
+      <c r="E10" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2" t="str">
+      <c r="C11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>pets</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="6" t="s">
         <v>28</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated posts. Added Created on
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\03_mindoffwork-posts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73484AF1-C32A-4077-A6C6-C6B765CFC42C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD92417-8BCA-4191-85A2-4082A98C2255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
   <si>
     <t>ID</t>
   </si>
@@ -267,6 +267,15 @@
   </si>
   <si>
     <t>#EBEAE5</t>
+  </si>
+  <si>
+    <t>Dive into the world of DIY furniture building using reclaimed wood.</t>
+  </si>
+  <si>
+    <t>#7DC5A1</t>
+  </si>
+  <si>
+    <t>CREATED_ON</t>
   </si>
 </sst>
 </file>
@@ -643,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE75069E-C97D-4B74-95E9-9740559F44A7}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -659,11 +668,11 @@
     <col min="6" max="6" width="57.26953125" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.7265625" style="1"/>
     <col min="8" max="8" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="1"/>
+    <col min="9" max="10" width="10.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -691,8 +700,11 @@
       <c r="I1" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -722,46 +734,52 @@
       <c r="I2" s="7">
         <v>45576</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2" s="7">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G3" s="1" t="str">
-        <f>LOWER(SUBSTITUTE(B3, " ", "-"))</f>
-        <v>diy-projects:-crafting-functional-furniture-from-reclaimed-wood</v>
+        <f t="shared" ref="G3:G11" si="0">LOWER(SUBSTITUTE(B3, " ", "-"))</f>
+        <v>the-future-of-smart-homes:-integrating-technology-for-a-seamless-lifestyle</v>
       </c>
       <c r="H3" s="4" t="str">
-        <f t="shared" ref="H3:H11" si="0">SUBSTITUTE(SUBSTITUTE(D3, "-", " "), ".", " ")</f>
-        <v>cardtoon style 3d minimalistic retro style app inside a phone surrounded by minimalists objects with green background jpeg</v>
+        <f t="shared" ref="H3:H11" si="1">SUBSTITUTE(SUBSTITUTE(D3, "-", " "), ".", " ")</f>
+        <v>cartoon illustration of windows laptop with grey background jpeg</v>
       </c>
       <c r="I3" s="7">
         <v>45576</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3" s="7">
+        <v>45568</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A11" si="1">A3+1</f>
+        <f t="shared" ref="A4:A11" si="2">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>60</v>
@@ -776,20 +794,23 @@
         <v>43</v>
       </c>
       <c r="G4" s="1" t="str">
-        <f>LOWER(SUBSTITUTE(B4, " ", "-"))</f>
-        <v>dive-into-the-world-of-diy-furniture-building-using-reclaimed-wood.-this-post-outlines-essential-tools-and-techniques,-plus-step-by-step-guides-to-create-beautiful,-sustainable-pieces-that-enhance-your-living-space-while-reducing-waste.</v>
+        <f t="shared" si="0"/>
+        <v>dive-into-the-world-of-diy-furniture-building-using-reclaimed-wood.</v>
       </c>
       <c r="H4" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cartoon illustration of simple small pond surounded by trees and rocks with mild blue background  jpeg</v>
       </c>
       <c r="I4" s="7">
         <v>45576</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J4" s="7">
+        <v>45568</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -808,20 +829,23 @@
         <v>44</v>
       </c>
       <c r="G5" s="1" t="str">
-        <f>LOWER(SUBSTITUTE(B5, " ", "-"))</f>
+        <f t="shared" si="0"/>
         <v>simplifying-your-life:-the-power-of-decluttering</v>
       </c>
       <c r="H5" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cartoon illustration of gray dslr style camera with mild orange background jpeg</v>
       </c>
       <c r="I5" s="7">
         <v>45576</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J5" s="7">
+        <v>45568</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -840,20 +864,23 @@
         <v>45</v>
       </c>
       <c r="G6" s="1" t="str">
-        <f>LOWER(SUBSTITUTE(B6, " ", "-"))</f>
+        <f t="shared" si="0"/>
         <v>the-joy-of-creating:-finding-your-artistic-voice</v>
       </c>
       <c r="H6" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cartoon illustration of coding themed image featuring git like logo command line interface with skyblue background jpeg</v>
       </c>
       <c r="I6" s="7">
         <v>45576</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J6" s="7">
+        <v>45572</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -872,20 +899,23 @@
         <v>46</v>
       </c>
       <c r="G7" s="1" t="str">
-        <f>LOWER(SUBSTITUTE(B7, " ", "-"))</f>
+        <f t="shared" si="0"/>
         <v>nourishing-simplicity:-wholesome-recipes-for-busy-lives</v>
       </c>
       <c r="H7" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cartoon illustration of small pond with lillypads and lotus in the middle surrounded by stones and plants with lavender background jpeg</v>
       </c>
       <c r="I7" s="7">
         <v>45576</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J7" s="7">
+        <v>45572</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -904,52 +934,58 @@
         <v>47</v>
       </c>
       <c r="G8" s="1" t="str">
-        <f>LOWER(SUBSTITUTE(B8, " ", "-"))</f>
+        <f t="shared" si="0"/>
         <v>streamlining-your-code:-best-practices-for-clean-programming</v>
       </c>
       <c r="H8" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cartoon illustration of smartphone homepage filled with app icons surrounded by random icons with yellow background jpeg</v>
       </c>
       <c r="I8" s="7">
         <v>45576</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J8" s="7">
+        <v>45572</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>48</v>
       </c>
       <c r="G9" s="1" t="str">
-        <f>LOWER(SUBSTITUTE(B9, " ", "-"))</f>
-        <v>the-future-of-smart-homes:-integrating-technology-for-a-seamless-lifestyle</v>
+        <f t="shared" si="0"/>
+        <v>diy-projects:-crafting-functional-furniture-from-reclaimed-wood</v>
       </c>
       <c r="H9" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>cartoon illustration of windows laptop with grey background jpeg</v>
+        <f t="shared" si="1"/>
+        <v>cardtoon style 3d minimalistic retro style app inside a phone surrounded by minimalists objects with green background jpeg</v>
       </c>
       <c r="I9" s="7">
         <v>45576</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J9" s="7">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -968,20 +1004,23 @@
         <v>49</v>
       </c>
       <c r="G10" s="1" t="str">
-        <f>LOWER(SUBSTITUTE(B10, " ", "-"))</f>
+        <f t="shared" si="0"/>
         <v>gardening-for-beginners:-cultivating-a-sustainable-home-garden</v>
       </c>
       <c r="H10" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cartoon illustration of gray dslr style camera with mild orange background jpeg</v>
       </c>
       <c r="I10" s="7">
         <v>45576</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J10" s="7">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1000,14 +1039,17 @@
         <v>50</v>
       </c>
       <c r="G11" s="1" t="str">
-        <f>LOWER(SUBSTITUTE(B11, " ", "-"))</f>
+        <f t="shared" si="0"/>
         <v>understanding-pet-behavior:-building-a-stronger-bond-with-your-furry-friends</v>
       </c>
       <c r="H11" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cardtoon style 3d minimalistic retro style app inside a phone surrounded by minimalists objects with green background jpeg</v>
       </c>
       <c r="I11" s="7">
+        <v>45576</v>
+      </c>
+      <c r="J11" s="7">
         <v>45576</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Home Posts and Restructured Dist export
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\03_mindoffwork-posts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\04_mindoff_filestorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD92417-8BCA-4191-85A2-4082A98C2255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9C9243-F190-428B-9106-DB625715665E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="topics" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="83">
   <si>
     <t>ID</t>
   </si>
@@ -276,12 +275,24 @@
   </si>
   <si>
     <t>CREATED_ON</t>
+  </si>
+  <si>
+    <t>IS_FEATURED</t>
+  </si>
+  <si>
+    <t>IS_POPULAR</t>
+  </si>
+  <si>
+    <t>IS_RECOMMENDED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -325,19 +336,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,404 +661,499 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE75069E-C97D-4B74-95E9-9740559F44A7}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="30.90625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="1"/>
-    <col min="4" max="4" width="29" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="1"/>
-    <col min="6" max="6" width="57.26953125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="1"/>
-    <col min="8" max="8" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.90625" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="6" max="6" width="57.26953125" customWidth="1"/>
+    <col min="8" max="8" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="10.08984375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="1" t="str">
+      <c r="G2" t="str">
         <f>LOWER(SUBSTITUTE(B2, " ", "-"))</f>
         <v>the-art-of-minimalism-in-modern-design</v>
       </c>
-      <c r="H2" s="4" t="str">
+      <c r="H2" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(D2, "-", " "), ".", " ")</f>
         <v>cartoon illustration of burger filled with onion lettuce meat patty cheese with teal background jpeg</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" s="5">
         <v>45576</v>
       </c>
-      <c r="J2" s="7">
+      <c r="M2" s="5">
         <v>45566</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="1" t="str">
+      <c r="G3" t="str">
         <f t="shared" ref="G3:G11" si="0">LOWER(SUBSTITUTE(B3, " ", "-"))</f>
         <v>the-future-of-smart-homes:-integrating-technology-for-a-seamless-lifestyle</v>
       </c>
-      <c r="H3" s="4" t="str">
+      <c r="H3" t="str">
         <f t="shared" ref="H3:H11" si="1">SUBSTITUTE(SUBSTITUTE(D3, "-", " "), ".", " ")</f>
         <v>cartoon illustration of windows laptop with grey background jpeg</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" s="5">
         <v>45576</v>
       </c>
-      <c r="J3" s="7">
+      <c r="M3" s="5">
         <v>45568</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4">
         <f t="shared" ref="A4:A11" si="2">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="1" t="str">
+      <c r="G4" t="str">
         <f t="shared" si="0"/>
         <v>dive-into-the-world-of-diy-furniture-building-using-reclaimed-wood.</v>
       </c>
-      <c r="H4" s="4" t="str">
+      <c r="H4" t="str">
         <f t="shared" si="1"/>
         <v>cartoon illustration of simple small pond surounded by trees and rocks with mild blue background  jpeg</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" s="5">
         <v>45576</v>
       </c>
-      <c r="J4" s="7">
+      <c r="M4" s="5">
         <v>45568</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="1" t="str">
+      <c r="G5" t="str">
         <f t="shared" si="0"/>
         <v>simplifying-your-life:-the-power-of-decluttering</v>
       </c>
-      <c r="H5" s="4" t="str">
+      <c r="H5" t="str">
         <f t="shared" si="1"/>
         <v>cartoon illustration of gray dslr style camera with mild orange background jpeg</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" s="5">
         <v>45576</v>
       </c>
-      <c r="J5" s="7">
+      <c r="M5" s="5">
         <v>45568</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="1" t="str">
+      <c r="G6" t="str">
         <f t="shared" si="0"/>
         <v>the-joy-of-creating:-finding-your-artistic-voice</v>
       </c>
-      <c r="H6" s="4" t="str">
+      <c r="H6" t="str">
         <f t="shared" si="1"/>
         <v>cartoon illustration of coding themed image featuring git like logo command line interface with skyblue background jpeg</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" s="5">
         <v>45576</v>
       </c>
-      <c r="J6" s="7">
+      <c r="M6" s="5">
         <v>45572</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="1" t="str">
+      <c r="G7" t="str">
         <f t="shared" si="0"/>
         <v>nourishing-simplicity:-wholesome-recipes-for-busy-lives</v>
       </c>
-      <c r="H7" s="4" t="str">
+      <c r="H7" t="str">
         <f t="shared" si="1"/>
         <v>cartoon illustration of small pond with lillypads and lotus in the middle surrounded by stones and plants with lavender background jpeg</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" s="5">
         <v>45576</v>
       </c>
-      <c r="J7" s="7">
+      <c r="M7" s="5">
         <v>45572</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>74</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="1" t="str">
+      <c r="G8" t="str">
         <f t="shared" si="0"/>
         <v>streamlining-your-code:-best-practices-for-clean-programming</v>
       </c>
-      <c r="H8" s="4" t="str">
+      <c r="H8" t="str">
         <f t="shared" si="1"/>
         <v>cartoon illustration of smartphone homepage filled with app icons surrounded by random icons with yellow background jpeg</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" s="5">
         <v>45576</v>
       </c>
-      <c r="J8" s="7">
+      <c r="M8" s="5">
         <v>45572</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="1" t="str">
+      <c r="G9" t="str">
         <f t="shared" si="0"/>
         <v>diy-projects:-crafting-functional-furniture-from-reclaimed-wood</v>
       </c>
-      <c r="H9" s="4" t="str">
+      <c r="H9" t="str">
         <f t="shared" si="1"/>
         <v>cardtoon style 3d minimalistic retro style app inside a phone surrounded by minimalists objects with green background jpeg</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" s="5">
         <v>45576</v>
       </c>
-      <c r="J9" s="7">
+      <c r="M9" s="5">
         <v>45576</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="1" t="str">
+      <c r="G10" t="str">
         <f t="shared" si="0"/>
         <v>gardening-for-beginners:-cultivating-a-sustainable-home-garden</v>
       </c>
-      <c r="H10" s="4" t="str">
+      <c r="H10" t="str">
         <f t="shared" si="1"/>
         <v>cartoon illustration of gray dslr style camera with mild orange background jpeg</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10" s="5">
         <v>45576</v>
       </c>
-      <c r="J10" s="7">
+      <c r="M10" s="5">
         <v>45576</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="1" t="str">
+      <c r="G11" t="str">
         <f t="shared" si="0"/>
         <v>understanding-pet-behavior:-building-a-stronger-bond-with-your-furry-friends</v>
       </c>
-      <c r="H11" s="4" t="str">
+      <c r="H11" t="str">
         <f t="shared" si="1"/>
         <v>cardtoon style 3d minimalistic retro style app inside a phone surrounded by minimalists objects with green background jpeg</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11" s="5">
         <v>45576</v>
       </c>
-      <c r="J11" s="7">
+      <c r="M11" s="5">
         <v>45576</v>
       </c>
     </row>
@@ -1081,217 +1185,215 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="4"/>
-    <col min="2" max="2" width="26.90625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.453125" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="4"/>
+    <col min="2" max="2" width="26.90625" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6" t="str">
+      <c r="C2" s="3" t="str">
         <f>LOWER(B2)</f>
         <v>design</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
+      <c r="A3" s="3">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="str">
+      <c r="C3" s="3" t="str">
         <f t="shared" ref="C3:C11" si="0">LOWER(B3)</f>
         <v>build</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
+      <c r="A4" s="3">
         <f>A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6" t="str">
+      <c r="C4" s="3" t="str">
         <f t="shared" si="0"/>
         <v>philosophy</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
+      <c r="A5" s="3">
         <f>A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6" t="str">
+      <c r="C5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>lifestyle</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
+      <c r="A6" s="3">
         <f>A5+1</f>
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="6" t="str">
+      <c r="C6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>artistry</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
+      <c r="A7" s="3">
         <f>A6+1</f>
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="6" t="str">
+      <c r="C7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>food</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
+      <c r="A8" s="3">
         <f t="shared" ref="A8:A11" si="1">A7+1</f>
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="6" t="str">
+      <c r="C8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>programming</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
+      <c r="A9" s="3">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="6" t="str">
+      <c r="C9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>tech</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="6">
+      <c r="A10" s="3">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="6" t="str">
+      <c r="C10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>gardening</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="6">
+      <c r="A11" s="3">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="6" t="str">
+      <c r="C11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>pets</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Altered topicslist.json to topics.json
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\04_mindoff_filestorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9C9243-F190-428B-9106-DB625715665E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD767F15-EA24-42B2-9942-8348B43E5D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
   <sheets>
     <sheet name="posts" sheetId="1" r:id="rId1"/>
@@ -663,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE75069E-C97D-4B74-95E9-9740559F44A7}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1179,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8A1887-075D-436C-B79D-D9001D13C034}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added Topics Url to Posts page
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\04_mindoff_filestorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD767F15-EA24-42B2-9942-8348B43E5D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442C56A7-25D1-4BE7-A5EE-6D05416FAE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
   <sheets>
     <sheet name="posts" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="84">
   <si>
     <t>ID</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>IS_RECOMMENDED</t>
+  </si>
+  <si>
+    <t>TOPIC_URL</t>
   </si>
 </sst>
 </file>
@@ -661,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE75069E-C97D-4B74-95E9-9740559F44A7}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -677,7 +680,7 @@
     <col min="9" max="13" width="10.08984375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -717,8 +720,11 @@
       <c r="M1" s="4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N1" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -760,8 +766,12 @@
       <c r="M2" s="5">
         <v>45566</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N2" t="str">
+        <f>VLOOKUP(C2, topics!B$2:D$100, 2, FALSE)</f>
+        <v>design</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -804,8 +814,12 @@
       <c r="M3" s="5">
         <v>45568</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N3" t="str">
+        <f>VLOOKUP(C3, topics!B$2:D$100, 2, FALSE)</f>
+        <v>programming</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" ref="A4:A11" si="2">A3+1</f>
         <v>3</v>
@@ -848,8 +862,12 @@
       <c r="M4" s="5">
         <v>45568</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N4" t="str">
+        <f>VLOOKUP(C4, topics!B$2:D$100, 2, FALSE)</f>
+        <v>design</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -892,8 +910,12 @@
       <c r="M5" s="5">
         <v>45568</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N5" t="str">
+        <f>VLOOKUP(C5, topics!B$2:D$100, 2, FALSE)</f>
+        <v>design</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -936,8 +958,12 @@
       <c r="M6" s="5">
         <v>45572</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N6" t="str">
+        <f>VLOOKUP(C6, topics!B$2:D$100, 2, FALSE)</f>
+        <v>design</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -980,8 +1006,12 @@
       <c r="M7" s="5">
         <v>45572</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N7" t="str">
+        <f>VLOOKUP(C7, topics!B$2:D$100, 2, FALSE)</f>
+        <v>design</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -1024,8 +1054,12 @@
       <c r="M8" s="5">
         <v>45572</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N8" t="str">
+        <f>VLOOKUP(C8, topics!B$2:D$100, 2, FALSE)</f>
+        <v>programming</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -1068,8 +1102,12 @@
       <c r="M9" s="5">
         <v>45576</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N9" t="str">
+        <f>VLOOKUP(C9, topics!B$2:D$100, 2, FALSE)</f>
+        <v>design</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -1112,8 +1150,12 @@
       <c r="M10" s="5">
         <v>45576</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N10" t="str">
+        <f>VLOOKUP(C10, topics!B$2:D$100, 2, FALSE)</f>
+        <v>programming</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -1155,6 +1197,10 @@
       </c>
       <c r="M11" s="5">
         <v>45576</v>
+      </c>
+      <c r="N11" t="str">
+        <f>VLOOKUP(C11, topics!B$2:D$100, 2, FALSE)</f>
+        <v>programming</v>
       </c>
     </row>
   </sheetData>
@@ -1179,8 +1225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8A1887-075D-436C-B79D-D9001D13C034}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Removed topic_url from posts sheet
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\04_mindoff_filestorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442C56A7-25D1-4BE7-A5EE-6D05416FAE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896A8FCF-CF26-43A0-AC47-0920AF29C382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="83">
   <si>
     <t>ID</t>
   </si>
@@ -284,9 +284,6 @@
   </si>
   <si>
     <t>IS_RECOMMENDED</t>
-  </si>
-  <si>
-    <t>TOPIC_URL</t>
   </si>
 </sst>
 </file>
@@ -664,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE75069E-C97D-4B74-95E9-9740559F44A7}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -680,7 +677,7 @@
     <col min="9" max="13" width="10.08984375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -720,11 +717,8 @@
       <c r="M1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -766,12 +760,8 @@
       <c r="M2" s="5">
         <v>45566</v>
       </c>
-      <c r="N2" t="str">
-        <f>VLOOKUP(C2, topics!B$2:D$100, 2, FALSE)</f>
-        <v>design</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -814,12 +804,8 @@
       <c r="M3" s="5">
         <v>45568</v>
       </c>
-      <c r="N3" t="str">
-        <f>VLOOKUP(C3, topics!B$2:D$100, 2, FALSE)</f>
-        <v>programming</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" ref="A4:A11" si="2">A3+1</f>
         <v>3</v>
@@ -862,12 +848,8 @@
       <c r="M4" s="5">
         <v>45568</v>
       </c>
-      <c r="N4" t="str">
-        <f>VLOOKUP(C4, topics!B$2:D$100, 2, FALSE)</f>
-        <v>design</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -910,12 +892,8 @@
       <c r="M5" s="5">
         <v>45568</v>
       </c>
-      <c r="N5" t="str">
-        <f>VLOOKUP(C5, topics!B$2:D$100, 2, FALSE)</f>
-        <v>design</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -958,12 +936,8 @@
       <c r="M6" s="5">
         <v>45572</v>
       </c>
-      <c r="N6" t="str">
-        <f>VLOOKUP(C6, topics!B$2:D$100, 2, FALSE)</f>
-        <v>design</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -1006,12 +980,8 @@
       <c r="M7" s="5">
         <v>45572</v>
       </c>
-      <c r="N7" t="str">
-        <f>VLOOKUP(C7, topics!B$2:D$100, 2, FALSE)</f>
-        <v>design</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -1054,12 +1024,8 @@
       <c r="M8" s="5">
         <v>45572</v>
       </c>
-      <c r="N8" t="str">
-        <f>VLOOKUP(C8, topics!B$2:D$100, 2, FALSE)</f>
-        <v>programming</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -1102,12 +1068,8 @@
       <c r="M9" s="5">
         <v>45576</v>
       </c>
-      <c r="N9" t="str">
-        <f>VLOOKUP(C9, topics!B$2:D$100, 2, FALSE)</f>
-        <v>design</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -1150,12 +1112,8 @@
       <c r="M10" s="5">
         <v>45576</v>
       </c>
-      <c r="N10" t="str">
-        <f>VLOOKUP(C10, topics!B$2:D$100, 2, FALSE)</f>
-        <v>programming</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -1197,10 +1155,6 @@
       </c>
       <c r="M11" s="5">
         <v>45576</v>
-      </c>
-      <c r="N11" t="str">
-        <f>VLOOKUP(C11, topics!B$2:D$100, 2, FALSE)</f>
-        <v>programming</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added posts export functionality
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\04_mindoff_filestorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896A8FCF-CF26-43A0-AC47-0920AF29C382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A8EFAF-7580-448F-8312-0401B86AE87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
@@ -663,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE75069E-C97D-4B74-95E9-9740559F44A7}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -738,7 +738,7 @@
         <v>40</v>
       </c>
       <c r="G2" t="str">
-        <f>LOWER(SUBSTITUTE(B2, " ", "-"))</f>
+        <f>LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B2, " ", "-"), ":", "-"), ";", "-"), ",", "-"), ".", "-"), "/", "-"))</f>
         <v>the-art-of-minimalism-in-modern-design</v>
       </c>
       <c r="H2" t="str">
@@ -782,8 +782,8 @@
         <v>42</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G11" si="0">LOWER(SUBSTITUTE(B3, " ", "-"))</f>
-        <v>the-future-of-smart-homes:-integrating-technology-for-a-seamless-lifestyle</v>
+        <f t="shared" ref="G3:G11" si="0">LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B3, " ", "-"), ":", "-"), ";", "-"), ",", "-"), ".", "-"), "/", "-"))</f>
+        <v>the-future-of-smart-homes--integrating-technology-for-a-seamless-lifestyle</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H11" si="1">SUBSTITUTE(SUBSTITUTE(D3, "-", " "), ".", " ")</f>
@@ -827,7 +827,7 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>dive-into-the-world-of-diy-furniture-building-using-reclaimed-wood.</v>
+        <v>dive-into-the-world-of-diy-furniture-building-using-reclaimed-wood-</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="1"/>
@@ -871,7 +871,7 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>simplifying-your-life:-the-power-of-decluttering</v>
+        <v>simplifying-your-life--the-power-of-decluttering</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="1"/>
@@ -915,7 +915,7 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>the-joy-of-creating:-finding-your-artistic-voice</v>
+        <v>the-joy-of-creating--finding-your-artistic-voice</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="1"/>
@@ -959,7 +959,7 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>nourishing-simplicity:-wholesome-recipes-for-busy-lives</v>
+        <v>nourishing-simplicity--wholesome-recipes-for-busy-lives</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="1"/>
@@ -1003,7 +1003,7 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>streamlining-your-code:-best-practices-for-clean-programming</v>
+        <v>streamlining-your-code--best-practices-for-clean-programming</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="1"/>
@@ -1047,7 +1047,7 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>diy-projects:-crafting-functional-furniture-from-reclaimed-wood</v>
+        <v>diy-projects--crafting-functional-furniture-from-reclaimed-wood</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="1"/>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>gardening-for-beginners:-cultivating-a-sustainable-home-garden</v>
+        <v>gardening-for-beginners--cultivating-a-sustainable-home-garden</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="1"/>
@@ -1135,7 +1135,7 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>understanding-pet-behavior:-building-a-stronger-bond-with-your-furry-friends</v>
+        <v>understanding-pet-behavior--building-a-stronger-bond-with-your-furry-friends</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Auto commit: 2024-10-14 02:06:58
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\04_mindoff_filestorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A8EFAF-7580-448F-8312-0401B86AE87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD13425B-D865-433F-9DEF-C0BBD773C1FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
@@ -268,9 +268,6 @@
     <t>#EBEAE5</t>
   </si>
   <si>
-    <t>Dive into the world of DIY furniture building using reclaimed wood.</t>
-  </si>
-  <si>
     <t>#7DC5A1</t>
   </si>
   <si>
@@ -284,6 +281,9 @@
   </si>
   <si>
     <t>IS_RECOMMENDED</t>
+  </si>
+  <si>
+    <t>Dive into the world of DIY furniture building using reclaimed wood</t>
   </si>
 </sst>
 </file>
@@ -664,7 +664,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -703,19 +703,19 @@
         <v>19</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>59</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -811,7 +811,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
         <v>60</v>
@@ -827,7 +827,7 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>dive-into-the-world-of-diy-furniture-building-using-reclaimed-wood-</v>
+        <v>dive-into-the-world-of-diy-furniture-building-using-reclaimed-wood</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="1"/>
@@ -1040,7 +1040,7 @@
         <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F9" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Auto commit: 2024-10-15 16:55:13
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\04_mindoff_filestorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD13425B-D865-433F-9DEF-C0BBD773C1FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC102A0-16B9-4267-8924-2A8B453094EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
@@ -663,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE75069E-C97D-4B74-95E9-9740559F44A7}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -673,6 +673,7 @@
     <col min="2" max="2" width="30.90625" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
     <col min="6" max="6" width="57.26953125" customWidth="1"/>
+    <col min="7" max="7" width="32.6328125" customWidth="1"/>
     <col min="8" max="8" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="9" max="13" width="10.08984375" style="5" bestFit="1" customWidth="1"/>
   </cols>
@@ -826,7 +827,7 @@
         <v>43</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" si="0"/>
+        <f>LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B4, " ", "-"), ":", "-"), ";", "-"), ",", "-"), ".", "-"), "/", "-"))</f>
         <v>dive-into-the-world-of-diy-furniture-building-using-reclaimed-wood</v>
       </c>
       <c r="H4" t="str">

</xml_diff>

<commit_message>
Auto commit: 2024-10-16 19:27:26
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\04_mindoff_filestorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC102A0-16B9-4267-8924-2A8B453094EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D62E1E-5D11-4DD4-BC3F-883877095786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="87">
   <si>
     <t>ID</t>
   </si>
@@ -284,6 +284,18 @@
   </si>
   <si>
     <t>Dive into the world of DIY furniture building using reclaimed wood</t>
+  </si>
+  <si>
+    <t>Quickly Integrate Tailwind CSS into an Existing Next.js App in Just 4 Steps</t>
+  </si>
+  <si>
+    <t>Recent versions of Next.js come packaged with Tailwind CSS, which we can enable during project creation. If you missed installing it out of the box, this guide will walk you through four simple steps to install and configure Tailwind CSS. Even though this post is tailored for Next.js, a similar method can be used to set up Tailwind in a React.js application as well.</t>
+  </si>
+  <si>
+    <t>minimalistic-cartoon-style-laptop-nextjs-app-tailwindcss-color-swatches-code-snippets-black-outline</t>
+  </si>
+  <si>
+    <t>#A2F9E9</t>
   </si>
 </sst>
 </file>
@@ -310,7 +322,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,8 +335,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -332,21 +356,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE75069E-C97D-4B74-95E9-9740559F44A7}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -675,487 +720,530 @@
     <col min="6" max="6" width="57.26953125" customWidth="1"/>
     <col min="7" max="7" width="32.6328125" customWidth="1"/>
     <col min="8" max="8" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="10.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="10.08984375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G2" t="str">
+      <c r="G2" s="7" t="str">
         <f>LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B2, " ", "-"), ":", "-"), ";", "-"), ",", "-"), ".", "-"), "/", "-"))</f>
         <v>the-art-of-minimalism-in-modern-design</v>
       </c>
-      <c r="H2" t="str">
+      <c r="H2" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(D2, "-", " "), ".", " ")</f>
         <v>cartoon illustration of burger filled with onion lettuce meat patty cheese with teal background jpeg</v>
       </c>
-      <c r="I2" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" s="5" t="b">
+      <c r="I2" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="K2" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2" s="5">
+      <c r="K2" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" s="8">
         <v>45576</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="8">
         <v>45566</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3">
+    <row r="3" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G3" t="str">
-        <f t="shared" ref="G3:G11" si="0">LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B3, " ", "-"), ":", "-"), ";", "-"), ",", "-"), ".", "-"), "/", "-"))</f>
+      <c r="G3" s="7" t="str">
+        <f t="shared" ref="G3:G12" si="0">LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B3, " ", "-"), ":", "-"), ";", "-"), ",", "-"), ".", "-"), "/", "-"))</f>
         <v>the-future-of-smart-homes--integrating-technology-for-a-seamless-lifestyle</v>
       </c>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H11" si="1">SUBSTITUTE(SUBSTITUTE(D3, "-", " "), ".", " ")</f>
+      <c r="H3" s="7" t="str">
+        <f t="shared" ref="H3:H12" si="1">SUBSTITUTE(SUBSTITUTE(D3, "-", " "), ".", " ")</f>
         <v>cartoon illustration of windows laptop with grey background jpeg</v>
       </c>
-      <c r="I3" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="5" t="b">
+      <c r="I3" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="K3" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L3" s="5">
+      <c r="K3" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" s="8">
         <v>45576</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="8">
         <v>45568</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4">
+    <row r="4" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7">
         <f t="shared" ref="A4:A11" si="2">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G4" t="str">
+      <c r="G4" s="7" t="str">
         <f>LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B4, " ", "-"), ":", "-"), ";", "-"), ",", "-"), ".", "-"), "/", "-"))</f>
         <v>dive-into-the-world-of-diy-furniture-building-using-reclaimed-wood</v>
       </c>
-      <c r="H4" t="str">
+      <c r="H4" s="7" t="str">
         <f t="shared" si="1"/>
         <v>cartoon illustration of simple small pond surounded by trees and rocks with mild blue background  jpeg</v>
       </c>
-      <c r="I4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L4" s="5">
+      <c r="I4" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" s="8">
         <v>45576</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="8">
         <v>45568</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5">
+    <row r="5" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G5" t="str">
+      <c r="G5" s="7" t="str">
         <f t="shared" si="0"/>
         <v>simplifying-your-life--the-power-of-decluttering</v>
       </c>
-      <c r="H5" t="str">
+      <c r="H5" s="7" t="str">
         <f t="shared" si="1"/>
         <v>cartoon illustration of gray dslr style camera with mild orange background jpeg</v>
       </c>
-      <c r="I5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L5" s="5">
+      <c r="I5" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" s="8">
         <v>45576</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="8">
         <v>45568</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="6" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G6" t="str">
+      <c r="G6" s="7" t="str">
         <f t="shared" si="0"/>
         <v>the-joy-of-creating--finding-your-artistic-voice</v>
       </c>
-      <c r="H6" t="str">
+      <c r="H6" s="7" t="str">
         <f t="shared" si="1"/>
         <v>cartoon illustration of coding themed image featuring git like logo command line interface with skyblue background jpeg</v>
       </c>
-      <c r="I6" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="5" t="b">
+      <c r="I6" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="K6" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" s="5">
+      <c r="K6" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" s="8">
         <v>45576</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="8">
         <v>45572</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7">
+    <row r="7" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G7" t="str">
+      <c r="G7" s="7" t="str">
         <f t="shared" si="0"/>
         <v>nourishing-simplicity--wholesome-recipes-for-busy-lives</v>
       </c>
-      <c r="H7" t="str">
+      <c r="H7" s="7" t="str">
         <f t="shared" si="1"/>
         <v>cartoon illustration of small pond with lillypads and lotus in the middle surrounded by stones and plants with lavender background jpeg</v>
       </c>
-      <c r="I7" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="5" t="b">
+      <c r="I7" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="K7" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L7" s="5">
+      <c r="K7" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" s="8">
         <v>45576</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="8">
         <v>45572</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8">
+    <row r="8" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G8" t="str">
+      <c r="G8" s="7" t="str">
         <f t="shared" si="0"/>
         <v>streamlining-your-code--best-practices-for-clean-programming</v>
       </c>
-      <c r="H8" t="str">
+      <c r="H8" s="7" t="str">
         <f t="shared" si="1"/>
         <v>cartoon illustration of smartphone homepage filled with app icons surrounded by random icons with yellow background jpeg</v>
       </c>
-      <c r="I8" s="5" t="b">
+      <c r="I8" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J8" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K8" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L8" s="5">
+      <c r="J8" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" s="8">
         <v>45576</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="8">
         <v>45572</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9">
+    <row r="9" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G9" t="str">
+      <c r="G9" s="7" t="str">
         <f t="shared" si="0"/>
         <v>diy-projects--crafting-functional-furniture-from-reclaimed-wood</v>
       </c>
-      <c r="H9" t="str">
+      <c r="H9" s="7" t="str">
         <f t="shared" si="1"/>
         <v>cardtoon style 3d minimalistic retro style app inside a phone surrounded by minimalists objects with green background jpeg</v>
       </c>
-      <c r="I9" s="5" t="b">
+      <c r="I9" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J9" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K9" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L9" s="5">
+      <c r="J9" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" s="8">
         <v>45576</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="8">
         <v>45576</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10">
+    <row r="10" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G10" t="str">
+      <c r="G10" s="7" t="str">
         <f t="shared" si="0"/>
         <v>gardening-for-beginners--cultivating-a-sustainable-home-garden</v>
       </c>
-      <c r="H10" t="str">
+      <c r="H10" s="7" t="str">
         <f t="shared" si="1"/>
         <v>cartoon illustration of gray dslr style camera with mild orange background jpeg</v>
       </c>
-      <c r="I10" s="5" t="b">
+      <c r="I10" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J10" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K10" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L10" s="5">
+      <c r="J10" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10" s="8">
         <v>45576</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="8">
         <v>45576</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11">
+    <row r="11" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G11" t="str">
+      <c r="G11" s="7" t="str">
         <f t="shared" si="0"/>
         <v>understanding-pet-behavior--building-a-stronger-bond-with-your-furry-friends</v>
       </c>
-      <c r="H11" t="str">
+      <c r="H11" s="7" t="str">
         <f t="shared" si="1"/>
         <v>cardtoon style 3d minimalistic retro style app inside a phone surrounded by minimalists objects with green background jpeg</v>
       </c>
-      <c r="I11" s="5" t="b">
+      <c r="I11" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J11" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K11" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L11" s="5">
+      <c r="J11" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11" s="8">
         <v>45576</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="8">
         <v>45576</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="9">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>quickly-integrate-tailwind-css-into-an-existing-next-js-app-in-just-4-steps</v>
+      </c>
+      <c r="H12" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>minimalistic cartoon style laptop nextjs app tailwindcss color swatches code snippets black outline</v>
+      </c>
+      <c r="I12" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" s="10">
+        <v>45581</v>
+      </c>
+      <c r="M12" s="10">
+        <v>45581</v>
       </c>
     </row>
   </sheetData>
@@ -1168,7 +1256,7 @@
           <x14:formula1>
             <xm:f>topics!$C$2:$C$1000</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C11</xm:sqref>
+          <xm:sqref>C2:C12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1193,72 +1281,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="str">
+      <c r="C2" s="2" t="str">
         <f>LOWER(B2)</f>
         <v>design</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="str">
+      <c r="C3" s="2" t="str">
         <f t="shared" ref="C3:C11" si="0">LOWER(B3)</f>
         <v>build</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <f>A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="str">
+      <c r="C4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>philosophy</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E4" t="s">
@@ -1266,18 +1354,18 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <f>A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="str">
+      <c r="C5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>lifestyle</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E5" t="s">
@@ -1285,18 +1373,18 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <f>A5+1</f>
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3" t="str">
+      <c r="C6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>artistry</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E6" t="s">
@@ -1304,18 +1392,18 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <f>A6+1</f>
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="str">
+      <c r="C7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>food</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E7" t="s">
@@ -1323,18 +1411,18 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <f t="shared" ref="A8:A11" si="1">A7+1</f>
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3" t="str">
+      <c r="C8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>programming</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E8" t="s">
@@ -1342,18 +1430,18 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="str">
+      <c r="C9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>tech</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E9" t="s">
@@ -1361,18 +1449,18 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="3" t="str">
+      <c r="C10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>gardening</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E10" t="s">
@@ -1380,18 +1468,18 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="3" t="str">
+      <c r="C11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>pets</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E11" t="s">

</xml_diff>

<commit_message>
Auto commit: 2024-10-16 19:43:59
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\04_mindoff_filestorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D62E1E-5D11-4DD4-BC3F-883877095786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23F9A4E-A998-4A2D-99BA-0F5076C847A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
@@ -292,10 +292,10 @@
     <t>Recent versions of Next.js come packaged with Tailwind CSS, which we can enable during project creation. If you missed installing it out of the box, this guide will walk you through four simple steps to install and configure Tailwind CSS. Even though this post is tailored for Next.js, a similar method can be used to set up Tailwind in a React.js application as well.</t>
   </si>
   <si>
-    <t>minimalistic-cartoon-style-laptop-nextjs-app-tailwindcss-color-swatches-code-snippets-black-outline</t>
-  </si>
-  <si>
     <t>#A2F9E9</t>
+  </si>
+  <si>
+    <t>minimalistic-cartoon-style-laptop-nextjs-app-tailwindcss-color-swatches-code-snippets-black-outline.jpeg</t>
   </si>
 </sst>
 </file>
@@ -708,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE75069E-C97D-4B74-95E9-9740559F44A7}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1214,10 +1214,10 @@
         <v>61</v>
       </c>
       <c r="D12" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>86</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>84</v>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="H12" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>minimalistic cartoon style laptop nextjs app tailwindcss color swatches code snippets black outline</v>
+        <v>minimalistic cartoon style laptop nextjs app tailwindcss color swatches code snippets black outline jpeg</v>
       </c>
       <c r="I12" s="11" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Auto commit: 2024-10-16 19:45:45
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\04_mindoff_filestorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23F9A4E-A998-4A2D-99BA-0F5076C847A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87449969-9A86-4816-8BE9-5BCBC1214D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
@@ -708,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE75069E-C97D-4B74-95E9-9740559F44A7}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1012,7 +1012,7 @@
         <v>cartoon illustration of small pond with lillypads and lotus in the middle surrounded by stones and plants with lavender background jpeg</v>
       </c>
       <c r="I7" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="8" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Auto commit: 2024-10-19 01:03:22
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\04_mindoff_filestorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87449969-9A86-4816-8BE9-5BCBC1214D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FEF356-DEB1-415A-9E33-F2CBD3B3A6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="topics" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="88">
   <si>
     <t>ID</t>
   </si>
@@ -296,6 +297,9 @@
   </si>
   <si>
     <t>minimalistic-cartoon-style-laptop-nextjs-app-tailwindcss-color-swatches-code-snippets-black-outline.jpeg</t>
+  </si>
+  <si>
+    <t>IS_GENERATE</t>
   </si>
 </sst>
 </file>
@@ -303,7 +307,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -383,15 +387,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE75069E-C97D-4B74-95E9-9740559F44A7}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -723,7 +727,7 @@
     <col min="9" max="13" width="10.08984375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -763,8 +767,11 @@
       <c r="M1" s="6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N1" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -806,8 +813,11 @@
       <c r="M2" s="8">
         <v>45566</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N2" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <f>A2+1</f>
         <v>2</v>
@@ -850,8 +860,11 @@
       <c r="M3" s="8">
         <v>45568</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N3" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <f t="shared" ref="A4:A11" si="2">A3+1</f>
         <v>3</v>
@@ -894,8 +907,11 @@
       <c r="M4" s="8">
         <v>45568</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N4" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -938,8 +954,11 @@
       <c r="M5" s="8">
         <v>45568</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N5" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -982,8 +1001,11 @@
       <c r="M6" s="8">
         <v>45572</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N6" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -1026,8 +1048,11 @@
       <c r="M7" s="8">
         <v>45572</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N7" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -1070,8 +1095,11 @@
       <c r="M8" s="8">
         <v>45572</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N8" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -1114,8 +1142,11 @@
       <c r="M9" s="8">
         <v>45576</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N9" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -1158,8 +1189,11 @@
       <c r="M10" s="8">
         <v>45576</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N10" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -1202,8 +1236,11 @@
       <c r="M11" s="8">
         <v>45576</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N11" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1244,6 +1281,9 @@
       </c>
       <c r="M12" s="10">
         <v>45581</v>
+      </c>
+      <c r="N12" s="8" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit: 2024-10-23 00:52:14
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\04_mindoff_filestorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FEF356-DEB1-415A-9E33-F2CBD3B3A6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDF1349-9436-4D2E-A22C-F5DC2B20485D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="topics" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="100">
   <si>
     <t>ID</t>
   </si>
@@ -161,9 +160,6 @@
     <t>Explore how minimalism influences contemporary design choices, from architecture to interior decor. Discover practical tips for incorporating minimalistic principles to create serene and functional spaces that prioritize simplicity and usability.</t>
   </si>
   <si>
-    <t>DIY Projects: Crafting Functional Furniture from Reclaimed Wood</t>
-  </si>
-  <si>
     <t>Dive into the world of DIY furniture building using reclaimed wood. This post outlines essential tools and techniques, plus step-by-step guides to create beautiful, sustainable pieces that enhance your living space while reducing waste.</t>
   </si>
   <si>
@@ -191,27 +187,6 @@
     <t>Explore the fascinating world of pet behavior and communication. This post offers insights into understanding your pet's needs and emotions, providing tips for strengthening the bond between you and your animal companions through positive reinforcement and care.</t>
   </si>
   <si>
-    <t>Understanding Pet Behavior: Building a Stronger Bond with Your Furry Friends</t>
-  </si>
-  <si>
-    <t>Gardening for Beginners: Cultivating a Sustainable Home Garden</t>
-  </si>
-  <si>
-    <t>The Future of Smart Homes: Integrating Technology for a Seamless Lifestyle</t>
-  </si>
-  <si>
-    <t>Streamlining Your Code: Best Practices for Clean Programming</t>
-  </si>
-  <si>
-    <t>Nourishing Simplicity: Wholesome Recipes for Busy Lives</t>
-  </si>
-  <si>
-    <t>The Joy of Creating: Finding Your Artistic Voice</t>
-  </si>
-  <si>
-    <t>Simplifying Your Life: The Power of Decluttering</t>
-  </si>
-  <si>
     <t>cartoon-illustration-of-small-pond-with-lillypads-and-lotus-in-the-middle-surrounded-by-stones-and-plants-with-lavender-background.jpeg</t>
   </si>
   <si>
@@ -284,12 +259,6 @@
     <t>IS_RECOMMENDED</t>
   </si>
   <si>
-    <t>Dive into the world of DIY furniture building using reclaimed wood</t>
-  </si>
-  <si>
-    <t>Quickly Integrate Tailwind CSS into an Existing Next.js App in Just 4 Steps</t>
-  </si>
-  <si>
     <t>Recent versions of Next.js come packaged with Tailwind CSS, which we can enable during project creation. If you missed installing it out of the box, this guide will walk you through four simple steps to install and configure Tailwind CSS. Even though this post is tailored for Next.js, a similar method can be used to set up Tailwind in a React.js application as well.</t>
   </si>
   <si>
@@ -300,6 +269,72 @@
   </si>
   <si>
     <t>IS_GENERATE</t>
+  </si>
+  <si>
+    <t>SUBTITLE</t>
+  </si>
+  <si>
+    <t>Add Tailwind CSS to Next.js</t>
+  </si>
+  <si>
+    <t>Quickly In 4 Steps</t>
+  </si>
+  <si>
+    <t>Understanding Pet Behavior</t>
+  </si>
+  <si>
+    <t>Building a Stronger Bond with Your Furry Friends</t>
+  </si>
+  <si>
+    <t>Gardening for Beginners</t>
+  </si>
+  <si>
+    <t>Cultivating a Sustainable Home Garden</t>
+  </si>
+  <si>
+    <t>DIY Projects</t>
+  </si>
+  <si>
+    <t>Functional Furniture from Reclaimed Wood</t>
+  </si>
+  <si>
+    <t>Best Practices for Clean Programming</t>
+  </si>
+  <si>
+    <t>Streamlining Your Code</t>
+  </si>
+  <si>
+    <t>Nourishing Simplicity</t>
+  </si>
+  <si>
+    <t>Wholesome Recipes for Busy Lives</t>
+  </si>
+  <si>
+    <t>The Joy of Creating</t>
+  </si>
+  <si>
+    <t>Finding Your Artistic Voice</t>
+  </si>
+  <si>
+    <t>Simplifying Your Life</t>
+  </si>
+  <si>
+    <t>Dive into the world of DIY furniture</t>
+  </si>
+  <si>
+    <t>Building using reclaimed wood</t>
+  </si>
+  <si>
+    <t>The Power of Decluttering</t>
+  </si>
+  <si>
+    <t>The Future of Smart Home</t>
+  </si>
+  <si>
+    <t>Integrating Technology for a Seamless Lifestyle</t>
+  </si>
+  <si>
+    <t>Transforming Spaces</t>
   </si>
 </sst>
 </file>
@@ -326,7 +361,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,12 +377,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,14 +422,55 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -710,24 +780,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE75069E-C97D-4B74-95E9-9740559F44A7}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.90625" customWidth="1"/>
-    <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="6" max="6" width="57.26953125" customWidth="1"/>
-    <col min="7" max="7" width="32.6328125" customWidth="1"/>
-    <col min="8" max="8" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="10.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.90625" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="7" max="7" width="57.26953125" customWidth="1"/>
+    <col min="8" max="8" width="32.6328125" customWidth="1"/>
+    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="10.08984375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -735,43 +805,46 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="J1" s="6" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -779,514 +852,552 @@
         <v>39</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="7" t="str">
-        <f>LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B2, " ", "-"), ":", "-"), ";", "-"), ",", "-"), ".", "-"), "/", "-"))</f>
-        <v>the-art-of-minimalism-in-modern-design</v>
-      </c>
       <c r="H2" s="7" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(D2, "-", " "), ".", " ")</f>
+        <f>LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(CONCATENATE(B2, C2), " ", "-"), ":", "-"), ";", "-"), ",", "-"), ".", "-"), "/", "-"))</f>
+        <v>the-art-of-minimalism-in-modern-designtransforming-spaces</v>
+      </c>
+      <c r="I2" s="7" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(E2, "-", " "), ".", " ")</f>
         <v>cartoon illustration of burger filled with onion lettuce meat patty cheese with teal background jpeg</v>
       </c>
-      <c r="I2" s="8" t="b">
-        <v>1</v>
-      </c>
       <c r="J2" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2" s="8">
+        <v>0</v>
+      </c>
+      <c r="L2" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" s="8">
         <v>45576</v>
       </c>
-      <c r="M2" s="8">
+      <c r="N2" s="8">
         <v>45566</v>
       </c>
-      <c r="N2" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="O2" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>75</v>
-      </c>
       <c r="E3" s="7" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="7" t="str">
-        <f t="shared" ref="G3:G12" si="0">LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B3, " ", "-"), ":", "-"), ";", "-"), ",", "-"), ".", "-"), "/", "-"))</f>
-        <v>the-future-of-smart-homes--integrating-technology-for-a-seamless-lifestyle</v>
+        <v>68</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="H3" s="7" t="str">
-        <f t="shared" ref="H3:H12" si="1">SUBSTITUTE(SUBSTITUTE(D3, "-", " "), ".", " ")</f>
+        <f t="shared" ref="H3:H12" si="0">LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(CONCATENATE(B3, C3), " ", "-"), ":", "-"), ";", "-"), ",", "-"), ".", "-"), "/", "-"))</f>
+        <v>the-future-of-smart-homeintegrating-technology-for-a-seamless-lifestyle</v>
+      </c>
+      <c r="I3" s="7" t="str">
+        <f t="shared" ref="I3:I12" si="1">SUBSTITUTE(SUBSTITUTE(E3, "-", " "), ".", " ")</f>
         <v>cartoon illustration of windows laptop with grey background jpeg</v>
       </c>
-      <c r="I3" s="8" t="b">
-        <v>1</v>
-      </c>
       <c r="J3" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="L3" s="8">
+        <v>0</v>
+      </c>
+      <c r="L3" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" s="8">
         <v>45576</v>
       </c>
-      <c r="M3" s="8">
+      <c r="N3" s="8">
         <v>45568</v>
       </c>
-      <c r="N3" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="O3" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <f t="shared" ref="A4:A11" si="2">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="7" t="str">
-        <f>LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B4, " ", "-"), ":", "-"), ";", "-"), ",", "-"), ".", "-"), "/", "-"))</f>
-        <v>dive-into-the-world-of-diy-furniture-building-using-reclaimed-wood</v>
+        <v>62</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="H4" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>dive-into-the-world-of-diy-furniturebuilding-using-reclaimed-wood</v>
+      </c>
+      <c r="I4" s="7" t="str">
         <f t="shared" si="1"/>
         <v>cartoon illustration of simple small pond surounded by trees and rocks with mild blue background  jpeg</v>
       </c>
-      <c r="I4" s="8" t="b">
-        <v>1</v>
-      </c>
       <c r="J4" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" s="8">
         <v>45576</v>
       </c>
-      <c r="M4" s="8">
+      <c r="N4" s="8">
         <v>45568</v>
       </c>
-      <c r="N4" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="O4" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="F5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="7" t="str">
+        <v>61</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>simplifying-your-life--the-power-of-decluttering</v>
-      </c>
-      <c r="H5" s="7" t="str">
+        <v>simplifying-your-lifethe-power-of-decluttering</v>
+      </c>
+      <c r="I5" s="7" t="str">
         <f t="shared" si="1"/>
         <v>cartoon illustration of gray dslr style camera with mild orange background jpeg</v>
       </c>
-      <c r="I5" s="8" t="b">
-        <v>1</v>
-      </c>
       <c r="J5" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" s="8">
         <v>45576</v>
       </c>
-      <c r="M5" s="8">
+      <c r="N5" s="8">
         <v>45568</v>
       </c>
-      <c r="N5" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="O5" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="7" t="str">
+        <v>64</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>the-joy-of-creating--finding-your-artistic-voice</v>
-      </c>
-      <c r="H6" s="7" t="str">
+        <v>the-joy-of-creatingfinding-your-artistic-voice</v>
+      </c>
+      <c r="I6" s="7" t="str">
         <f t="shared" si="1"/>
         <v>cartoon illustration of coding themed image featuring git like logo command line interface with skyblue background jpeg</v>
       </c>
-      <c r="I6" s="8" t="b">
-        <v>1</v>
-      </c>
       <c r="J6" s="8" t="b">
         <v>0</v>
       </c>
       <c r="K6" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" s="8">
+        <v>0</v>
+      </c>
+      <c r="L6" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" s="8">
         <v>45576</v>
       </c>
-      <c r="M6" s="8">
+      <c r="N6" s="8">
         <v>45572</v>
       </c>
-      <c r="N6" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="O6" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="7" t="str">
+        <v>54</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>nourishing-simplicity--wholesome-recipes-for-busy-lives</v>
-      </c>
-      <c r="H7" s="7" t="str">
+        <v>nourishing-simplicitywholesome-recipes-for-busy-lives</v>
+      </c>
+      <c r="I7" s="7" t="str">
         <f t="shared" si="1"/>
         <v>cartoon illustration of small pond with lillypads and lotus in the middle surrounded by stones and plants with lavender background jpeg</v>
       </c>
-      <c r="I7" s="8" t="b">
-        <v>0</v>
-      </c>
       <c r="J7" s="8" t="b">
         <v>0</v>
       </c>
       <c r="K7" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="L7" s="8">
+        <v>0</v>
+      </c>
+      <c r="L7" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" s="8">
         <v>45576</v>
       </c>
-      <c r="M7" s="8">
+      <c r="N7" s="8">
         <v>45572</v>
       </c>
-      <c r="N7" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="O7" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="7" t="str">
+        <v>66</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>streamlining-your-code--best-practices-for-clean-programming</v>
-      </c>
-      <c r="H8" s="7" t="str">
+        <v>best-practices-for-clean-programmingstreamlining-your-code</v>
+      </c>
+      <c r="I8" s="7" t="str">
         <f t="shared" si="1"/>
         <v>cartoon illustration of smartphone homepage filled with app icons surrounded by random icons with yellow background jpeg</v>
       </c>
-      <c r="I8" s="8" t="b">
-        <v>0</v>
-      </c>
       <c r="J8" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" s="8">
         <v>45576</v>
       </c>
-      <c r="M8" s="8">
+      <c r="N8" s="8">
         <v>45572</v>
       </c>
-      <c r="N8" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="O8" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>diy-projects--crafting-functional-furniture-from-reclaimed-wood</v>
+        <v>69</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="H9" s="7" t="str">
+        <f>LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(CONCATENATE(B9, C9), " ", "-"), ":", "-"), ";", "-"), ",", "-"), ".", "-"), "/", "-"))</f>
+        <v>functional-furniture-from-reclaimed-wooddiy-projects</v>
+      </c>
+      <c r="I9" s="7" t="str">
         <f t="shared" si="1"/>
         <v>cardtoon style 3d minimalistic retro style app inside a phone surrounded by minimalists objects with green background jpeg</v>
       </c>
-      <c r="I9" s="8" t="b">
-        <v>0</v>
-      </c>
       <c r="J9" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="L9" s="8">
-        <v>45576</v>
+      <c r="L9" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="M9" s="8">
         <v>45576</v>
       </c>
-      <c r="N9" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N9" s="8">
+        <v>45576</v>
+      </c>
+      <c r="O9" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="7" t="str">
+      <c r="G10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>gardening-for-beginners--cultivating-a-sustainable-home-garden</v>
-      </c>
-      <c r="H10" s="7" t="str">
+        <v>gardening-for-beginnerscultivating-a-sustainable-home-garden</v>
+      </c>
+      <c r="I10" s="7" t="str">
         <f t="shared" si="1"/>
         <v>cartoon illustration of gray dslr style camera with mild orange background jpeg</v>
       </c>
-      <c r="I10" s="8" t="b">
-        <v>0</v>
-      </c>
       <c r="J10" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="L10" s="8">
-        <v>45576</v>
+      <c r="L10" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="M10" s="8">
         <v>45576</v>
       </c>
-      <c r="N10" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N10" s="8">
+        <v>45576</v>
+      </c>
+      <c r="O10" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="7" t="str">
+        <v>56</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>understanding-pet-behavior--building-a-stronger-bond-with-your-furry-friends</v>
-      </c>
-      <c r="H11" s="7" t="str">
+        <v>understanding-pet-behaviorbuilding-a-stronger-bond-with-your-furry-friends</v>
+      </c>
+      <c r="I11" s="7" t="str">
         <f t="shared" si="1"/>
         <v>cardtoon style 3d minimalistic retro style app inside a phone surrounded by minimalists objects with green background jpeg</v>
       </c>
-      <c r="I11" s="8" t="b">
-        <v>0</v>
-      </c>
       <c r="J11" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="L11" s="8">
-        <v>45576</v>
+      <c r="L11" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="M11" s="8">
         <v>45576</v>
       </c>
-      <c r="N11" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N11" s="8">
+        <v>45576</v>
+      </c>
+      <c r="O11" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12" s="9" t="str">
+        <v>75</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>quickly-integrate-tailwind-css-into-an-existing-next-js-app-in-just-4-steps</v>
-      </c>
-      <c r="H12" s="9" t="str">
+        <v>add-tailwind-css-to-next-jsquickly-in-4-steps</v>
+      </c>
+      <c r="I12" s="9" t="str">
         <f t="shared" si="1"/>
         <v>minimalistic cartoon style laptop nextjs app tailwindcss color swatches code snippets black outline jpeg</v>
       </c>
-      <c r="I12" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="L12" s="10">
-        <v>45581</v>
+      <c r="J12" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="M12" s="10">
         <v>45581</v>
       </c>
-      <c r="N12" s="8" t="b">
+      <c r="N12" s="10">
+        <v>45581</v>
+      </c>
+      <c r="O12" s="10" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J1:L1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -1296,7 +1407,7 @@
           <x14:formula1>
             <xm:f>topics!$C$2:$C$1000</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C12</xm:sqref>
+          <xm:sqref>D2:D12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Auto commit: 2024-10-23 01:06:18
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\04_mindoff_filestorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDF1349-9436-4D2E-A22C-F5DC2B20485D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F928E06-4394-4BA7-A1D0-EA377E49BD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="101">
   <si>
     <t>ID</t>
   </si>
@@ -205,9 +205,6 @@
     <t>cardtoon-style-3d-minimalistic-retro-style-app-inside-a-phone-surrounded-by-minimalists-objects-with-green-background.jpeg</t>
   </si>
   <si>
-    <t>#70BB9A</t>
-  </si>
-  <si>
     <t>cartoon-illustration-of-burger-filled-with-onion-lettuce-meat-patty-cheese-with-teal-background.jpeg</t>
   </si>
   <si>
@@ -335,6 +332,12 @@
   </si>
   <si>
     <t>Transforming Spaces</t>
+  </si>
+  <si>
+    <t>kid-petting-a-dog-with-yellow-background.jpeg</t>
+  </si>
+  <si>
+    <t>#FCF2D7</t>
   </si>
 </sst>
 </file>
@@ -783,7 +786,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -805,7 +808,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -826,22 +829,22 @@
         <v>19</v>
       </c>
       <c r="J1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>73</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>51</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -852,16 +855,16 @@
         <v>39</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>52</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>40</v>
@@ -899,19 +902,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>98</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>53</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>67</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>68</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>41</v>
@@ -949,19 +952,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>52</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>42</v>
@@ -999,19 +1002,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>52</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>43</v>
@@ -1049,19 +1052,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>52</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>44</v>
@@ -1099,10 +1102,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>52</v>
@@ -1149,19 +1152,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>53</v>
       </c>
       <c r="E8" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>66</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>46</v>
@@ -1199,10 +1202,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>52</v>
@@ -1211,7 +1214,7 @@
         <v>55</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>47</v>
@@ -1249,19 +1252,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>84</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>53</v>
       </c>
       <c r="E10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>48</v>
@@ -1299,19 +1302,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>53</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>49</v>
@@ -1322,7 +1325,7 @@
       </c>
       <c r="I11" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>cardtoon style 3d minimalistic retro style app inside a phone surrounded by minimalists objects with green background jpeg</v>
+        <v>kid petting a dog with yellow background jpeg</v>
       </c>
       <c r="J11" s="8" t="b">
         <v>0</v>
@@ -1348,22 +1351,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>53</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H12" s="9" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Auto commit: 2024-10-23 01:17:10
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\04_mindoff_filestorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F928E06-4394-4BA7-A1D0-EA377E49BD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32602CF9-2BA6-4186-BE0D-E5F7747E2262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
@@ -208,9 +208,6 @@
     <t>cartoon-illustration-of-burger-filled-with-onion-lettuce-meat-patty-cheese-with-teal-background.jpeg</t>
   </si>
   <si>
-    <t>#B9E3D5</t>
-  </si>
-  <si>
     <t>cartoon-illustration-of-coding-themed-image-featuring-git-like-logo-command-line-interface-with-skyblue-background.jpeg</t>
   </si>
   <si>
@@ -226,9 +223,6 @@
     <t>cartoon-illustration-of-simple-small-pond-surounded-by-trees-and-rocks-with-mild-blue-background-.jpeg</t>
   </si>
   <si>
-    <t>#A5F6E3</t>
-  </si>
-  <si>
     <t>cartoon-illustration-of-smartphone-homepage-filled-with-app-icons-surrounded-by-random-icons-with-yellow-background.jpeg</t>
   </si>
   <si>
@@ -259,9 +253,6 @@
     <t>Recent versions of Next.js come packaged with Tailwind CSS, which we can enable during project creation. If you missed installing it out of the box, this guide will walk you through four simple steps to install and configure Tailwind CSS. Even though this post is tailored for Next.js, a similar method can be used to set up Tailwind in a React.js application as well.</t>
   </si>
   <si>
-    <t>#A2F9E9</t>
-  </si>
-  <si>
     <t>minimalistic-cartoon-style-laptop-nextjs-app-tailwindcss-color-swatches-code-snippets-black-outline.jpeg</t>
   </si>
   <si>
@@ -338,6 +329,15 @@
   </si>
   <si>
     <t>#FCF2D7</t>
+  </si>
+  <si>
+    <t>#C7CCEC</t>
+  </si>
+  <si>
+    <t>#C2D7CE</t>
+  </si>
+  <si>
+    <t>#BBE6DD</t>
   </si>
 </sst>
 </file>
@@ -786,7 +786,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -808,7 +808,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -829,22 +829,22 @@
         <v>19</v>
       </c>
       <c r="J1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>72</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>51</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -855,7 +855,7 @@
         <v>39</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>52</v>
@@ -864,7 +864,7 @@
         <v>56</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>40</v>
@@ -902,19 +902,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>53</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>41</v>
@@ -952,19 +952,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>52</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>42</v>
@@ -1002,19 +1002,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>52</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>60</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>43</v>
@@ -1052,19 +1052,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>52</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>44</v>
@@ -1102,10 +1102,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>52</v>
@@ -1152,19 +1152,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>53</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>46</v>
@@ -1202,10 +1202,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>52</v>
@@ -1214,7 +1214,7 @@
         <v>55</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>47</v>
@@ -1252,19 +1252,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>53</v>
       </c>
       <c r="E10" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>60</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>48</v>
@@ -1302,19 +1302,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>53</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>49</v>
@@ -1351,22 +1351,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>53</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H12" s="9" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Auto commit: 2024-10-23 16:57:52
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\04_mindoff_filestorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32602CF9-2BA6-4186-BE0D-E5F7747E2262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F0372D-DC19-4467-B3C2-BC460B93F6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="topics" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -411,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -425,14 +426,13 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -440,36 +440,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -785,22 +755,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE75069E-C97D-4B74-95E9-9740559F44A7}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.90625" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.85546875" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="7" max="7" width="57.26953125" customWidth="1"/>
-    <col min="8" max="8" width="32.6328125" customWidth="1"/>
-    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="10.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.28515625" customWidth="1"/>
+    <col min="8" max="8" width="32.5703125" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="10.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -847,7 +817,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -878,7 +848,7 @@
         <v>cartoon illustration of burger filled with onion lettuce meat patty cheese with teal background jpeg</v>
       </c>
       <c r="J2" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="8" t="b">
         <v>0</v>
@@ -896,7 +866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <f>A2+1</f>
         <v>2</v>
@@ -928,7 +898,7 @@
         <v>cartoon illustration of windows laptop with grey background jpeg</v>
       </c>
       <c r="J3" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" s="8" t="b">
         <v>0</v>
@@ -946,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <f t="shared" ref="A4:A11" si="2">A3+1</f>
         <v>3</v>
@@ -996,7 +966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -1046,7 +1016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -1096,7 +1066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -1146,7 +1116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -1196,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -1246,7 +1216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -1296,7 +1266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -1346,7 +1316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1426,15 +1396,15 @@
       <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.90625" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.453125" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1451,7 +1421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1469,7 +1439,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>A2+1</f>
         <v>2</v>
@@ -1488,7 +1458,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>A3+1</f>
         <v>3</v>
@@ -1507,7 +1477,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>A4+1</f>
         <v>4</v>
@@ -1526,7 +1496,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>A5+1</f>
         <v>5</v>
@@ -1545,7 +1515,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>A6+1</f>
         <v>6</v>
@@ -1564,7 +1534,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" ref="A8:A11" si="1">A7+1</f>
         <v>7</v>
@@ -1583,7 +1553,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -1602,7 +1572,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1621,7 +1591,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="1"/>
         <v>10</v>

</xml_diff>

<commit_message>
Auto commit: 2024-10-23 17:00:46
</commit_message>
<xml_diff>
--- a/db_sheet.xlsx
+++ b/db_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Work\01_Mindoff\01_Projects\04_mindoff_filestorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F0372D-DC19-4467-B3C2-BC460B93F6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D878154-3178-4732-9737-0603F769B1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D32074DA-35A3-4FC7-862B-75C4005D81AF}"/>
   </bookViews>
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE75069E-C97D-4B74-95E9-9740559F44A7}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,8 +1097,8 @@
         <f t="shared" si="1"/>
         <v>cartoon illustration of small pond with lillypads and lotus in the middle surrounded by stones and plants with lavender background jpeg</v>
       </c>
-      <c r="J7" s="8" t="b">
-        <v>0</v>
+      <c r="J7" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="K7" s="8" t="b">
         <v>0</v>

</xml_diff>